<commit_message>
TODO: likers and reposters - validate if not None
</commit_message>
<xml_diff>
--- a/groups_Ivan.xlsx
+++ b/groups_Ivan.xlsx
@@ -552,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -563,7 +563,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
data prep script added
</commit_message>
<xml_diff>
--- a/groups_Ivan.xlsx
+++ b/groups_Ivan.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -219,7 +219,7 @@
     <t>Сегмент</t>
   </si>
   <si>
-    <t>Id</t>
+    <t>group_id</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -563,7 +563,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>